<commit_message>
19th August 2022 - Session
</commit_message>
<xml_diff>
--- a/exambook.xlsx
+++ b/exambook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\cetpa\exambook_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2B8D99-775E-4349-A05E-3D4693516447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB42CB0-2380-4276-9B38-D8BA5D3B7157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DB Table" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="182">
   <si>
     <t>Types of login - candidate &lt; teachers &lt; admin</t>
   </si>
@@ -435,9 +435,6 @@
     <t>num_questions</t>
   </si>
   <si>
-    <t>[1,20,2,40,5,15]</t>
-  </si>
-  <si>
     <t>subject1</t>
   </si>
   <si>
@@ -502,6 +499,90 @@
   </si>
   <si>
     <t>pass_status</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>negativemarking</t>
+  </si>
+  <si>
+    <t>[{'1', 10}, {'4', 15}, {'5', 20}]</t>
+  </si>
+  <si>
+    <t>examlog_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/questions/getquestionbysubject?subject=1&amp;count=10</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/createexam</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/updateexam</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/removeexam/exam_id</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/fetchallexams</t>
+  </si>
+  <si>
+    <t>INT AUTOINCREMENT NOT NULL</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>DEFAULT - timestamp</t>
+  </si>
+  <si>
+    <t>exams</t>
+  </si>
+  <si>
+    <t>examlog</t>
+  </si>
+  <si>
+    <t>examlog_details</t>
+  </si>
+  <si>
+    <t>strart exam</t>
+  </si>
+  <si>
+    <t>array/json</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/startexam</t>
+  </si>
+  <si>
+    <t>BODY - examid, userid, questions</t>
+  </si>
+  <si>
+    <t>end of exam</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/updateexam</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/listallexams</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/listallexamsbyuserid</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/listallexamsbyexamid</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/getallexamlogbyexamid</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/saveexamentry</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/examlog/updateexamentry</t>
   </si>
 </sst>
 </file>
@@ -533,7 +614,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +645,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -578,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -596,6 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -911,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598E409D-B184-44C1-9772-DD09FE403E30}">
-  <dimension ref="C2:R30"/>
+  <dimension ref="C2:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,12 +1022,12 @@
     <col min="13" max="13" width="16.44140625" customWidth="1"/>
     <col min="14" max="14" width="18.5546875" customWidth="1"/>
     <col min="15" max="15" width="3.109375" style="11" customWidth="1"/>
-    <col min="16" max="16" width="19.88671875" customWidth="1"/>
-    <col min="17" max="17" width="17.21875" customWidth="1"/>
-    <col min="18" max="18" width="3.109375" style="11" customWidth="1"/>
+    <col min="16" max="18" width="19.88671875" customWidth="1"/>
+    <col min="19" max="19" width="17.21875" customWidth="1"/>
+    <col min="20" max="20" width="3.109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:20" x14ac:dyDescent="0.3">
       <c r="I2" t="s">
         <v>127</v>
       </c>
@@ -950,7 +1038,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
@@ -981,12 +1069,14 @@
       <c r="P3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R3" s="10"/>
-    </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="S3" s="1"/>
+      <c r="T3" s="10"/>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1011,14 +1101,17 @@
       <c r="N4" t="s">
         <v>128</v>
       </c>
-      <c r="P4" t="s">
-        <v>128</v>
+      <c r="P4" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="Q4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="R4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1043,14 +1136,17 @@
       <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="P5" t="s">
-        <v>20</v>
+      <c r="P5" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="Q5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="R5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1069,14 +1165,17 @@
       <c r="M6" t="s">
         <v>130</v>
       </c>
-      <c r="P6" t="s">
-        <v>149</v>
+      <c r="P6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="Q6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="R6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1090,19 +1189,19 @@
         <v>94</v>
       </c>
       <c r="M7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N7" t="s">
         <v>144</v>
-      </c>
-      <c r="N7" t="s">
-        <v>145</v>
       </c>
       <c r="P7" t="s">
         <v>131</v>
       </c>
-      <c r="Q7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="R7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>24</v>
       </c>
@@ -1119,13 +1218,13 @@
         <v>82</v>
       </c>
       <c r="P8" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="R8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>26</v>
       </c>
@@ -1139,13 +1238,16 @@
         <v>85</v>
       </c>
       <c r="M9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="R9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C10" s="9" t="s">
         <v>32</v>
       </c>
@@ -1158,11 +1260,14 @@
       <c r="G10" t="s">
         <v>85</v>
       </c>
+      <c r="M10" t="s">
+        <v>154</v>
+      </c>
       <c r="P10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>39</v>
       </c>
@@ -1178,11 +1283,14 @@
       <c r="I11" t="s">
         <v>96</v>
       </c>
+      <c r="M11" t="s">
+        <v>155</v>
+      </c>
       <c r="P11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>35</v>
       </c>
@@ -1196,10 +1304,10 @@
         <v>97</v>
       </c>
       <c r="P12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>36</v>
@@ -1213,8 +1321,14 @@
       <c r="I13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" t="s">
         <v>37</v>
@@ -1228,8 +1342,14 @@
       <c r="I14" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>38</v>
       </c>
@@ -1243,7 +1363,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>62</v>
       </c>
@@ -1267,12 +1387,12 @@
         <v>82</v>
       </c>
       <c r="N18" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M21" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N21" s="14">
         <v>4</v>
@@ -1280,7 +1400,7 @@
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M22" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N22" s="14">
         <v>30</v>
@@ -1290,49 +1410,49 @@
       <c r="C23" s="7"/>
       <c r="D23" s="4"/>
       <c r="M23" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N23" s="14"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M24" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N24" s="14"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M25" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N25" s="14"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M26" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N26" s="14"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M27" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N27" s="14"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M28" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N28" s="14"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M29" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N29" s="14"/>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.3">
       <c r="M30" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N30" s="14"/>
     </row>
@@ -1489,32 +1609,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBCD982-A1F7-4F12-9554-A4111D34D39C}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="57.5546875" customWidth="1"/>
-    <col min="7" max="7" width="43.77734375" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="57.5546875" customWidth="1"/>
+    <col min="8" max="8" width="43.77734375" customWidth="1"/>
+    <col min="9" max="9" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1524,184 +1644,396 @@
       <c r="C3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="4" t="s">
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="4" t="s">
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="2" t="s">
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="4" t="s">
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="12"/>
+      <c r="I7" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="4" t="s">
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="4">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="4">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="G12" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="H12" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="4" t="s">
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="4">
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="G13" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="H13" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="4" t="s">
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="4">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="4" t="s">
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="4">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="4" t="s">
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="4">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="4" t="s">
+    <row r="17" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="4">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="G17" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="4">
+        <v>13</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" t="s">
+        <v>170</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="H28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>24</v>
+      </c>
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{CF5B090D-923E-4F39-A190-24B68A4A347A}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{5FE462A3-D5BF-4639-9BF6-C95D99F65B44}"/>
-    <hyperlink ref="F7" r:id="rId3" xr:uid="{D0EBD89A-D66D-4DE7-86DF-5DFE6CF72550}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{18C25863-A0B6-42AA-9649-2C7EF3D9B6E3}"/>
-    <hyperlink ref="F5" r:id="rId5" xr:uid="{3B0BBC9D-C2D9-4372-8F28-57C51CE84779}"/>
-    <hyperlink ref="F12" r:id="rId6" xr:uid="{23D62CBE-F913-48E1-BB61-011CC1B0AF3A}"/>
-    <hyperlink ref="F13" r:id="rId7" xr:uid="{5D7C7235-0931-41A4-8D9C-A25FED980A75}"/>
-    <hyperlink ref="F14" r:id="rId8" xr:uid="{6E5D5C64-149F-469D-8FC2-C6D6F15B429A}"/>
-    <hyperlink ref="F15" r:id="rId9" xr:uid="{690443BB-935C-4306-975F-AD350037CCE8}"/>
-    <hyperlink ref="F16" r:id="rId10" xr:uid="{35BFFB03-C142-47BD-897D-7983C61F6FCE}"/>
-    <hyperlink ref="F17" r:id="rId11" xr:uid="{A6AD5FE8-090D-469D-B831-49F3D53948E1}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{CF5B090D-923E-4F39-A190-24B68A4A347A}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{5FE462A3-D5BF-4639-9BF6-C95D99F65B44}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{D0EBD89A-D66D-4DE7-86DF-5DFE6CF72550}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{18C25863-A0B6-42AA-9649-2C7EF3D9B6E3}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{3B0BBC9D-C2D9-4372-8F28-57C51CE84779}"/>
+    <hyperlink ref="G12" r:id="rId6" xr:uid="{23D62CBE-F913-48E1-BB61-011CC1B0AF3A}"/>
+    <hyperlink ref="G13" r:id="rId7" xr:uid="{5D7C7235-0931-41A4-8D9C-A25FED980A75}"/>
+    <hyperlink ref="G14" r:id="rId8" xr:uid="{6E5D5C64-149F-469D-8FC2-C6D6F15B429A}"/>
+    <hyperlink ref="G15" r:id="rId9" xr:uid="{690443BB-935C-4306-975F-AD350037CCE8}"/>
+    <hyperlink ref="G16" r:id="rId10" xr:uid="{35BFFB03-C142-47BD-897D-7983C61F6FCE}"/>
+    <hyperlink ref="G17" r:id="rId11" xr:uid="{A6AD5FE8-090D-469D-B831-49F3D53948E1}"/>
+    <hyperlink ref="G18" r:id="rId12" xr:uid="{CCA6D8DB-6FD6-4F1E-A6BE-E9998F49A666}"/>
+    <hyperlink ref="G21" r:id="rId13" xr:uid="{6109F10E-4576-4415-B406-F68219381D40}"/>
+    <hyperlink ref="G22" r:id="rId14" xr:uid="{9C5634F0-C9F8-4B88-A0AA-706ED21ABF4B}"/>
+    <hyperlink ref="G23" r:id="rId15" xr:uid="{FAD1C03F-B1EF-4ABB-8A5F-2A12BC735068}"/>
+    <hyperlink ref="G24" r:id="rId16" xr:uid="{3090E6DB-7D8A-4D87-A17A-9FEE3668328F}"/>
+    <hyperlink ref="G28" r:id="rId17" xr:uid="{F5E4AD3E-3D29-43F8-9921-DD385159694D}"/>
+    <hyperlink ref="G29" r:id="rId18" xr:uid="{38EE0906-4D73-48CA-BB79-459BE0D18733}"/>
+    <hyperlink ref="G30" r:id="rId19" xr:uid="{76A465A1-2A64-4AD6-9462-F3475E232513}"/>
+    <hyperlink ref="G31" r:id="rId20" xr:uid="{9090ACE3-7488-43F2-AF9E-709555B56FFA}"/>
+    <hyperlink ref="G32" r:id="rId21" xr:uid="{09D485E2-72A0-4C25-92E2-C9F87E5076F4}"/>
+    <hyperlink ref="G37" r:id="rId22" xr:uid="{E6480310-DFDD-4A01-9339-50A9D8BA425D}"/>
+    <hyperlink ref="G38" r:id="rId23" xr:uid="{40F1FD9F-D824-4FB2-8699-A5249DC0476F}"/>
+    <hyperlink ref="G39" r:id="rId24" xr:uid="{C5C45D3B-9415-478A-A3BE-08B79D6F9C69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>